<commit_message>
Updated excel file and Base file with ome up headless feature
</commit_message>
<xml_diff>
--- a/src/main/java/com/excel/lib/util/SampleExcel.xlsx
+++ b/src/main/java/com/excel/lib/util/SampleExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arijitdas\eclipse-workspace\Appium_Assignment\src\main\java\com\excel\lib\util\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E133E405-8DAD-4F7C-8086-191EA17FD9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E8EFF9-6AA1-44AD-B60A-9239924E0CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E78FF5EA-6506-4A74-9AE1-4C827656B31E}"/>
+    <workbookView xWindow="2120" yWindow="2120" windowWidth="14400" windowHeight="7270" xr2:uid="{E78FF5EA-6506-4A74-9AE1-4C827656B31E}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleExcel" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>PLATFORM_NAME</t>
   </si>
@@ -77,6 +77,18 @@
   </si>
   <si>
     <t>com.example.android.apis.ApiDemos</t>
+  </si>
+  <si>
+    <t>headless</t>
+  </si>
+  <si>
+    <t>start_with_code</t>
+  </si>
+  <si>
+    <t>start_manually</t>
+  </si>
+  <si>
+    <t>manual</t>
   </si>
 </sst>
 </file>
@@ -128,12 +140,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -451,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D518643-E7D1-4AAD-A3A7-9BF663F1D610}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,6 +534,22 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{708D1B70-E130-4956-9F48-6C2BFC89841A}"/>

</xml_diff>